<commit_message>
created new ebs metrics script to take less inputs
</commit_message>
<xml_diff>
--- a/data/input_ebs_volumes.xlsx
+++ b/data/input_ebs_volumes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grmeri/repos/aws/aws-cw-augment/aws-get-ebs-metrics/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grmeri/repos/aws/aws-storage-get-metrics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E0377D-F63D-7D4C-8B6F-204FEB8F011A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817A02C6-E930-E34D-B6C8-C6863E4A750A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="10080" windowWidth="43180" windowHeight="16260" activeTab="1" xr2:uid="{7BF96EA4-294C-3041-AD8B-25A51595320B}"/>
+    <workbookView xWindow="8720" yWindow="12540" windowWidth="43180" windowHeight="16260" activeTab="1" xr2:uid="{7BF96EA4-294C-3041-AD8B-25A51595320B}"/>
   </bookViews>
   <sheets>
     <sheet name="EC2 instances" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
   <si>
     <t>ap-southeast-1</t>
   </si>
@@ -41,9 +41,6 @@
     <t>region</t>
   </si>
   <si>
-    <t>r5.large</t>
-  </si>
-  <si>
     <t>ap-southeast-2</t>
   </si>
   <si>
@@ -98,28 +95,31 @@
     <t>vol_side</t>
   </si>
   <si>
-    <t>inst001-backup001</t>
-  </si>
-  <si>
-    <t>inst001-data001</t>
-  </si>
-  <si>
-    <t>inst001</t>
-  </si>
-  <si>
-    <t>inst001-log001</t>
-  </si>
-  <si>
-    <t>i-0d719e7fdhjhj233</t>
-  </si>
-  <si>
-    <t>vol-0992e4cd0edafdd12</t>
-  </si>
-  <si>
-    <t>vol-0683825422632624f</t>
-  </si>
-  <si>
-    <t>vol-0be158c486bf2282e</t>
+    <t>i-072e21af1a822d3f1</t>
+  </si>
+  <si>
+    <t>vol-03d0f3d58730c3fd4</t>
+  </si>
+  <si>
+    <t>i-07a82f460153a799b</t>
+  </si>
+  <si>
+    <t>r6a.xlarge</t>
+  </si>
+  <si>
+    <t>k8s_02</t>
+  </si>
+  <si>
+    <t>k8s_01</t>
+  </si>
+  <si>
+    <t>vol-02e9f0e75fc3b7750</t>
+  </si>
+  <si>
+    <t>vol01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -606,277 +606,277 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -890,7 +890,7 @@
   <dimension ref="A1:K719"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,51 +908,51 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>200</v>
@@ -961,33 +961,33 @@
         <v>3000</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>100</v>
@@ -996,51 +996,30 @@
         <v>3000</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
-      <c r="G4">
-        <v>3000</v>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="673" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>